<commit_message>
tests acceptation sur la page panier et mise à jour du code avec des messages d'alerte !
</commit_message>
<xml_diff>
--- a/DW_P5_Plan_tests_acceptation.xlsx
+++ b/DW_P5_Plan_tests_acceptation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\P5_ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF604D51-5CEB-4525-9410-8D2FC46445F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2A3B8C-88BB-4733-9587-928D7AACF976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
     <t>OK / Description erreur : La communication avec l'API n'est pas établie et les produits ne peuvent pas être affichés. L'utilisateur est averti de l'echec de connexion par un message d'alerte.</t>
   </si>
   <si>
@@ -81,6 +78,36 @@
   </si>
   <si>
     <t>OK / Si l'utilisateur cherche à outrepasser la limite fixée, un message d'alerte le rappelera à l'ordre ! Si celui-là insiste dans sa démarche, l'envoi de l'article dans le panier restera impossible !</t>
+  </si>
+  <si>
+    <t>Le clic sur le lien panier du menu</t>
+  </si>
+  <si>
+    <t>Tous les produits du panier de l'utilisateur sont affichés sur la page cart avec le détail de la couleur et de la quantité choisie (que l'utilisateur peut encore changer grâce à un input de type Number).</t>
+  </si>
+  <si>
+    <t>ouvre la page cart qui liste tous les produits que l'utilisateur a ajoutés à son panier</t>
+  </si>
+  <si>
+    <t>Un Input de type Number permet à l'utilisateur de changer la quantité d'un produit.</t>
+  </si>
+  <si>
+    <t>OK / Si l'utilisateur cherche à outrepasser la limite fixée, un message d'alerte le rappelera à l'ordre ! La quantité de l'article dans le Localstorage ne pourra pas franchir le plafond de 100.</t>
+  </si>
+  <si>
+    <t>Sur la page cart, l'utilisateur peut changer la quantité d'un produit.</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton Supprimer ou décrémenter l'Input de type Number jusqu'à 0</t>
+  </si>
+  <si>
+    <t>Supprimer un produit du panier.</t>
+  </si>
+  <si>
+    <t>Le produit est supprimé du localstorage et du DOM. Les valeurs totales de quantités et de prix sont mises à jour sur la page panier.</t>
+  </si>
+  <si>
+    <t>OK / Une alerte est générée pour valider la suppression de l'article si l'Input a une valeur de 0.</t>
   </si>
 </sst>
 </file>
@@ -629,8 +656,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -670,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.5">
@@ -678,16 +705,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
@@ -695,44 +722,68 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="5" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
       <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="64.8" x14ac:dyDescent="0.5">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A8" s="12"/>

</xml_diff>

<commit_message>
Messages de confirmation de suppression d'un article, lorsque la quantité est à 0, et au clic sur le bouton supprimer !
</commit_message>
<xml_diff>
--- a/DW_P5_Plan_tests_acceptation.xlsx
+++ b/DW_P5_Plan_tests_acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2A3B8C-88BB-4733-9587-928D7AACF976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B2F4FE-4944-45F8-A791-2B63ED239F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
plan d'acceptation, message de suppression d'article
</commit_message>
<xml_diff>
--- a/DW_P5_Plan_tests_acceptation.xlsx
+++ b/DW_P5_Plan_tests_acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B2F4FE-4944-45F8-A791-2B63ED239F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0837A312-AF04-4CE0-83D5-56AAEDFA92C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>Un Input de type Number permet à l'utilisateur de changer la quantité d'un produit.</t>
   </si>
   <si>
-    <t>OK / Si l'utilisateur cherche à outrepasser la limite fixée, un message d'alerte le rappelera à l'ordre ! La quantité de l'article dans le Localstorage ne pourra pas franchir le plafond de 100.</t>
-  </si>
-  <si>
     <t>Sur la page cart, l'utilisateur peut changer la quantité d'un produit.</t>
   </si>
   <si>
@@ -107,7 +104,10 @@
     <t>Le produit est supprimé du localstorage et du DOM. Les valeurs totales de quantités et de prix sont mises à jour sur la page panier.</t>
   </si>
   <si>
-    <t>OK / Une alerte est générée pour valider la suppression de l'article si l'Input a une valeur de 0.</t>
+    <t>OK / Si l'utilisateur cherche à outrepasser la limite fixée, un message d'alerte le rappelera à l'ordre ! La quantité de l'article dans le Localstorage ne pourra pas franchir le plafond de 100. Sur la page, la quantité sera initialisée à 100.</t>
+  </si>
+  <si>
+    <t>OK / Une message de confirmation est générée pour valider la suppression de l'article. En cas de décrémentation de l'Input jusqu'à 0, si l'utilisateur ne valide pas la suppression, la quantité du produit est réinitialisée à 1.</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -751,12 +751,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" ht="151.19999999999999" x14ac:dyDescent="0.5">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>19</v>
@@ -765,21 +765,21 @@
         <v>14</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="64.8" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Plan tests acceptation, reste la page confirmation. Restauration du backend dans son état d'origine
</commit_message>
<xml_diff>
--- a/DW_P5_Plan_tests_acceptation.xlsx
+++ b/DW_P5_Plan_tests_acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0837A312-AF04-4CE0-83D5-56AAEDFA92C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C3C72E-5BEB-4AE7-918D-0378BE70B858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>OK / Une message de confirmation est générée pour valider la suppression de l'article. En cas de décrémentation de l'Input jusqu'à 0, si l'utilisateur ne valide pas la suppression, la quantité du produit est réinitialisée à 1.</t>
+  </si>
+  <si>
+    <t>Un formulaire permet à l'utilisateur de valider la commande !</t>
+  </si>
+  <si>
+    <t>La validité des données rentrées dans les champs du formulaire est testée en direct, et une seconde fois lors du clic sur le bouton "Commander !"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si les champs du formulaire sont tous valides, la commande peut être envoyée après un message de confirmation comportant un récapitulatif des données du formulaire, du nombre d'articles commandés, ainsi que le prix total.  </t>
+  </si>
+  <si>
+    <t>OK / Si la connexion avec l'API ne peut être établie, l'utilisateur en sera informé par un message d'alerte. Si le panier est vide, l'utilisateur sera informé par une alerte de l'impossibilité de passer la commande.</t>
   </si>
 </sst>
 </file>
@@ -656,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -785,12 +797,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
       <c r="A8" s="12"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A9" s="12"/>

</xml_diff>

<commit_message>
Vérification des commentaires des fonctions.
</commit_message>
<xml_diff>
--- a/DW_P5_Plan_tests_acceptation.xlsx
+++ b/DW_P5_Plan_tests_acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C3C72E-5BEB-4AE7-918D-0378BE70B858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7C9B2-52E0-4DF2-A1DF-A9A61D7EC21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finalisation du plan tests d'acceptation
</commit_message>
<xml_diff>
--- a/DW_P5_Plan_tests_acceptation.xlsx
+++ b/DW_P5_Plan_tests_acceptation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openclassrooms\Form_Dev_Web\projet_5\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7C9B2-52E0-4DF2-A1DF-A9A61D7EC21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4F5BC2-1916-4ED2-9A90-B4FB5FAE873F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -120,6 +120,42 @@
   </si>
   <si>
     <t>OK / Si la connexion avec l'API ne peut être établie, l'utilisateur en sera informé par un message d'alerte. Si le panier est vide, l'utilisateur sera informé par une alerte de l'impossibilité de passer la commande.</t>
+  </si>
+  <si>
+    <t>Si la commande est validée par l'utilisateur, ce dernier est redirigé vers la page confirmation.html</t>
+  </si>
+  <si>
+    <t>L'API renvoie en réponse, les informations entrées par l'utilisateur, les informations des articles commandés ainsi que le numéro de commande (orderId). L'orderId est passé dans l'URL de la page confirmation</t>
+  </si>
+  <si>
+    <t>Dans la page confirmation.html, l'orderId est récupéré dans l'URL, et est affiché sur la page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK / Si la connexion avec l'API ne peut être établie, l'utilisateur en sera informé par un message d'alerte. </t>
+  </si>
+  <si>
+    <t>Si la commande est passée, le localStorage est vidé de tous les articles,</t>
+  </si>
+  <si>
+    <t>Le succès du passage de la commande provoque la redirection vers la page confirmation.html ainsi que la vidange du localStorage de tous les articles.</t>
+  </si>
+  <si>
+    <t>Reinitialisation du localStorage.</t>
+  </si>
+  <si>
+    <t>OK / Des problèmes de connexion avec l'API peuvent bloquer la commande.</t>
+  </si>
+  <si>
+    <t>Dans la page confirmation.html, suppression des informations concernant orderId</t>
+  </si>
+  <si>
+    <t>Après récupération de orderId dans l'URL, orderId est effacé de l'instance de l'objet URL.</t>
+  </si>
+  <si>
+    <t>Suppression de orderId de l'instance de l'objet URL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK / </t>
   </si>
 </sst>
 </file>
@@ -668,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -798,7 +834,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
-      <c r="A8" s="12"/>
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
       <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
@@ -812,26 +850,54 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="12"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A10" s="12"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="86.4" x14ac:dyDescent="0.5">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="64.8" x14ac:dyDescent="0.5">
       <c r="A11" s="12"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
+      <c r="B11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A12" s="12"/>

</xml_diff>